<commit_message>
create tab 13 report
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_13_rpt_CF_PortfolioSummary.xlsx
+++ b/backend/reports/xlsx/Tab_13_rpt_CF_PortfolioSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleshapka/Development/github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEB01642-6807-1B4A-8235-1F636A1FCEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EC877A-0013-1B43-9355-3124CE13DE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34560" windowHeight="19700" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,40 +36,167 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>{#date=d.date}</t>
   </si>
   <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+    <t>{$r.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$r1}</t>
+  </si>
+  <si>
+    <t>CO #</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Descoped</t>
+  </si>
+  <si>
+    <t>{$p.co_number}</t>
+  </si>
+  <si>
+    <t>{$p.start_date}</t>
+  </si>
+  <si>
+    <t>{$p.end_date}</t>
+  </si>
+  <si>
+    <t>{$p.project_number}</t>
+  </si>
+  <si>
+    <t>{$p.status}</t>
+  </si>
+  <si>
+    <t>{$p.total_fee_amount}</t>
+  </si>
+  <si>
+    <t>{$p.total_expense_amount}</t>
+  </si>
+  <si>
+    <t>{$p.remaining}</t>
+  </si>
+  <si>
+    <t>{$p.descoped}</t>
+  </si>
+  <si>
+    <t>{$t.total_fee_amount}</t>
+  </si>
+  <si>
+    <t>{#p = d.reportsByPortfolioWithTotals[i].projects[i]}</t>
+  </si>
+  <si>
+    <t>{#p1 = d.reportsByPortfolioWithTotals[i].projects[i+1]}</t>
+  </si>
+  <si>
+    <t>{#r = d.reportsByPortfolioWithTotals[i]}</t>
+  </si>
+  <si>
+    <t>{#r1 = d.reportsByPortfolioWithTotals[i+1]}</t>
+  </si>
+  <si>
+    <t>{#s = d.reportsByPortfolioWithTotals.portfolio_totals}</t>
+  </si>
+  <si>
+    <t>{$s.total_fee_amount}</t>
+  </si>
+  <si>
+    <t>{$s.total_expense_amount}</t>
+  </si>
+  <si>
+    <t>{$s.remaining}</t>
+  </si>
+  <si>
+    <t>{$s.descoped}</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>GDX Division Totals</t>
+  </si>
+  <si>
+    <t>{#t = d.grandTotals[0]}</t>
+  </si>
+  <si>
+    <t>{$t.total_expense_amount}</t>
+  </si>
+  <si>
+    <t>{$t.remaining}</t>
+  </si>
+  <si>
+    <t>{$t.descoped}</t>
+  </si>
+  <si>
+    <t>{$p1.co_number}</t>
+  </si>
+  <si>
+    <t>Portfolio Contract Summary for {$fy} as of {$date}</t>
+  </si>
+  <si>
+    <t>Maximum Amount</t>
+  </si>
+  <si>
+    <t>{$p.maximum_amount}</t>
+  </si>
+  <si>
+    <t>{$s.maximum_amount}</t>
+  </si>
+  <si>
+    <t>{$t.maximum_amount}</t>
+  </si>
+  <si>
+    <t>Invoiced to Date</t>
+  </si>
+  <si>
+    <t>{$p.invoiced_to_date}</t>
+  </si>
+  <si>
+    <t>{$s.invoiced_to_date}</t>
+  </si>
+  <si>
+    <t>{$t.invoiced_to_date}</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>{$p.supplier_name}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="m/dd/yy;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,11 +229,28 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,30 +335,22 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="medium">
         <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -224,9 +366,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -239,12 +378,36 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,8 +441,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2411614</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -623,113 +786,260 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="3" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="C3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="17" thickBot="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19">
+      <c r="A9" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="19">
+      <c r="A10" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="19">
+      <c r="A11" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="19">
+      <c r="A12" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="19">
+      <c r="A13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" ht="19">
+      <c r="A14" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="19">
+      <c r="A15" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="19">
+      <c r="A16" s="19"/>
+    </row>
+    <row r="17" spans="1:1" ht="19">
+      <c r="A17" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="19">
+      <c r="A18" s="19" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>

</xml_diff>